<commit_message>
Clean datasets for use in further analysis
</commit_message>
<xml_diff>
--- a/clean_yr_nrg_price_indices.xlsx
+++ b/clean_yr_nrg_price_indices.xlsx
@@ -370,27 +370,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>us_ex_rate</t>
+          <t>us.dollar.exchange.rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ppp</t>
+          <t>purchasing.power.parities</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ppi</t>
+          <t>producer.price.index</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cpi</t>
+          <t>consumer.price.index</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cpi_nrg</t>
+          <t>cpi.energy</t>
         </is>
       </c>
     </row>

</xml_diff>